<commit_message>
Correción de unos errores mínimos
</commit_message>
<xml_diff>
--- a/exports/volumen.xlsx
+++ b/exports/volumen.xlsx
@@ -3098,7 +3098,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3148,7 +3148,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -6379,7 +6379,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -6402,7 +6402,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -6425,7 +6425,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -6448,7 +6448,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -6471,7 +6471,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -9694,7 +9694,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D377" t="inlineStr">
@@ -9719,7 +9719,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
@@ -9744,7 +9744,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -9769,7 +9769,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
@@ -9794,7 +9794,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
@@ -13069,7 +13069,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D512" t="inlineStr">
@@ -13094,7 +13094,7 @@
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D513" t="inlineStr">
@@ -13119,7 +13119,7 @@
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D514" t="inlineStr">
@@ -13144,7 +13144,7 @@
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D515" t="inlineStr">
@@ -13169,7 +13169,7 @@
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D516" t="inlineStr">
@@ -16444,7 +16444,7 @@
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
@@ -16469,7 +16469,7 @@
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -16494,7 +16494,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D649" t="inlineStr">
@@ -16519,7 +16519,7 @@
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D650" t="inlineStr">
@@ -16544,7 +16544,7 @@
       </c>
       <c r="C651" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D651" t="inlineStr">
@@ -19829,7 +19829,7 @@
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D782" t="inlineStr">
@@ -19854,7 +19854,7 @@
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D783" t="inlineStr">
@@ -19879,7 +19879,7 @@
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D784" t="inlineStr">
@@ -19906,7 +19906,7 @@
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D785" t="inlineStr">
@@ -19931,7 +19931,7 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>019</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D786" t="inlineStr">

</xml_diff>